<commit_message>
Added licensing to samples
</commit_message>
<xml_diff>
--- a/Minimum Viable Security Program/Example Documents/Vendor AI Assessment.xlsx
+++ b/Minimum Viable Security Program/Example Documents/Vendor AI Assessment.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541E124D-78AE-42DF-8A4D-8C7FB82F6B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790016DD-715F-40DD-8CC6-812541B48078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11925" yWindow="885" windowWidth="34500" windowHeight="19365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8940" yWindow="2895" windowWidth="17025" windowHeight="18180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AI Risk in SaaS Vendors" sheetId="2" r:id="rId1"/>
+    <sheet name="License" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Category</t>
   </si>
@@ -107,12 +108,21 @@
   <si>
     <t>5.3  Do you have processes to detect, correct, and communicate AI errors, bias, or unintended behavior?</t>
   </si>
+  <si>
+    <t>© SafetyLight LLC — Released under CC0 1.0 Universal (Public Domain Dedication).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provided as-is, without any warranty or guarantee of suitability. Customize before use. </t>
+  </si>
+  <si>
+    <t>Original available on GitHub.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +175,14 @@
       <sz val="12"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -297,8 +315,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -348,14 +367,15 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -648,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8FE8A6-71D3-45A4-97B2-1B92EC528B99}">
   <dimension ref="A1:EZ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
@@ -708,16 +728,15 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:156" s="18" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:156" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
       <c r="C4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:156" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
@@ -989,7 +1008,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:7" s="18" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="9"/>
       <c r="C17" s="12" t="s">
@@ -998,9 +1017,8 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="9"/>
       <c r="C18" s="12" t="s">
@@ -1010,72 +1028,72 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -1345,4 +1363,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1864DDBA-C7C6-4BF5-9D5D-0A3CE16988E0}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="80.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{1D18BAE8-F1F8-4605-ACD0-1B7A2DDD9E7A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>